<commit_message>
google filter text trial
</commit_message>
<xml_diff>
--- a/com.verizon/src/test/resources/test_data_verizon.xlsx
+++ b/com.verizon/src/test/resources/test_data_verizon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.verizon/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8EE842-D80F-CE44-AB0C-FC4BD3642B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DCBC99-440D-D645-8D53-7C085B2AF026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16140" xr2:uid="{98B19BF0-E3A6-844B-87BE-D61402A4F806}"/>
   </bookViews>
@@ -399,7 +399,7 @@
   <dimension ref="A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
trade in device test case setup
</commit_message>
<xml_diff>
--- a/com.verizon/src/test/resources/test_data_verizon.xlsx
+++ b/com.verizon/src/test/resources/test_data_verizon.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.verizon/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3BCBF4-8768-414B-9C7D-E6155E1EB503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4DA068-BA3F-F646-9B85-3E89E62A79CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="1" xr2:uid="{98B19BF0-E3A6-844B-87BE-D61402A4F806}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="3" xr2:uid="{98B19BF0-E3A6-844B-87BE-D61402A4F806}"/>
   </bookViews>
   <sheets>
     <sheet name="Google5GPhones" sheetId="1" r:id="rId1"/>
     <sheet name="PhoneOfChoice" sheetId="2" r:id="rId2"/>
     <sheet name="Smartwatches" sheetId="3" r:id="rId3"/>
+    <sheet name="TradeInDevice" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Google</t>
   </si>
@@ -59,6 +60,36 @@
   </si>
   <si>
     <t>has been added to cart.</t>
+  </si>
+  <si>
+    <t>brands</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>LG</t>
+  </si>
+  <si>
+    <t>Motorola</t>
+  </si>
+  <si>
+    <t>HTC</t>
+  </si>
+  <si>
+    <t>OnePlus</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>Nokia</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -439,7 +470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F25CBE0-7FD2-F340-85B8-B97390FEE2A1}">
   <dimension ref="A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -498,4 +529,77 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AEDE32-A5FE-AC41-8BC4-115B4CE0E9A2}">
+  <dimension ref="A2:A12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
working on trade in test case
</commit_message>
<xml_diff>
--- a/com.verizon/src/test/resources/test_data_verizon.xlsx
+++ b/com.verizon/src/test/resources/test_data_verizon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.verizon/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5151C2-3845-B645-B9A5-195BCAC8B36E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A804AE-6914-DD48-B050-2053843E65C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="3" xr2:uid="{98B19BF0-E3A6-844B-87BE-D61402A4F806}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16060" activeTab="4" xr2:uid="{98B19BF0-E3A6-844B-87BE-D61402A4F806}"/>
   </bookViews>
   <sheets>
     <sheet name="Google5GPhones" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>Google</t>
   </si>
@@ -63,47 +63,32 @@
     <t>has been added to cart.</t>
   </si>
   <si>
-    <t>brands</t>
-  </si>
-  <si>
-    <t>Apple</t>
-  </si>
-  <si>
     <t>Samsung</t>
   </si>
   <si>
-    <t>LG</t>
-  </si>
-  <si>
-    <t>Motorola</t>
-  </si>
-  <si>
-    <t>HTC</t>
-  </si>
-  <si>
-    <t>OnePlus</t>
-  </si>
-  <si>
-    <t>Microsoft</t>
-  </si>
-  <si>
-    <t>Nokia</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Apple iPhone 8 Plus, 64GB Gray</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -115,6 +100,10 @@
       <sz val="11"/>
       <name val="Menlo"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,10 +126,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,7 +476,7 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -520,7 +511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36D147A-E162-B54D-A1C4-FABABDCAA153}">
   <dimension ref="A2:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -558,10 +549,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>3</v>
@@ -580,71 +571,75 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AEDE32-A5FE-AC41-8BC4-115B4CE0E9A2}">
-  <dimension ref="A2:A12"/>
+  <dimension ref="A2:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2" customWidth="1"/>
+    <col min="2" max="7" width="10.83203125" style="2"/>
+    <col min="8" max="8" width="37.33203125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>16</v>
-      </c>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test view apple tablets passed
</commit_message>
<xml_diff>
--- a/com.verizon/src/test/resources/test_data_verizon.xlsx
+++ b/com.verizon/src/test/resources/test_data_verizon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.verizon/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD362A4-12AF-E446-BD6E-80455B0BB9C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E365D2-D890-E440-A1D0-2AC8EF15A1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16060" activeTab="4" xr2:uid="{98B19BF0-E3A6-844B-87BE-D61402A4F806}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16060" activeTab="5" xr2:uid="{98B19BF0-E3A6-844B-87BE-D61402A4F806}"/>
   </bookViews>
   <sheets>
     <sheet name="Google5GPhones" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="PhoneOfChoice" sheetId="2" r:id="rId3"/>
     <sheet name="Smartwatches" sheetId="3" r:id="rId4"/>
     <sheet name="TradeInDevice" sheetId="7" r:id="rId5"/>
+    <sheet name="AppleTablets" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>Google</t>
   </si>
@@ -79,6 +80,9 @@
   </si>
   <si>
     <t>Apple iPhone 8 Plus, 64GB Gray</t>
+  </si>
+  <si>
+    <t>Shop Apple tablets</t>
   </si>
 </sst>
 </file>
@@ -564,20 +568,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EF569BC-D8F0-7F42-B31A-9C34490EC750}">
   <dimension ref="A2:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="10.83203125" style="2"/>
+    <col min="1" max="5" width="10.83203125" style="2"/>
+    <col min="6" max="6" width="10.83203125" style="2" customWidth="1"/>
     <col min="7" max="7" width="28" style="2" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -596,6 +601,29 @@
       </c>
       <c r="G2" s="2" t="s">
         <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7505121-C4A8-6E43-B005-E9FA764849C8}">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test compare hotspots passed
</commit_message>
<xml_diff>
--- a/com.verizon/src/test/resources/test_data_verizon.xlsx
+++ b/com.verizon/src/test/resources/test_data_verizon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.verizon/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E365D2-D890-E440-A1D0-2AC8EF15A1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B5FFB0-665C-8749-9F9F-9947568B58D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16060" activeTab="5" xr2:uid="{98B19BF0-E3A6-844B-87BE-D61402A4F806}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16060" activeTab="7" xr2:uid="{98B19BF0-E3A6-844B-87BE-D61402A4F806}"/>
   </bookViews>
   <sheets>
     <sheet name="Google5GPhones" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="Smartwatches" sheetId="3" r:id="rId4"/>
     <sheet name="TradeInDevice" sheetId="7" r:id="rId5"/>
     <sheet name="AppleTablets" sheetId="8" r:id="rId6"/>
+    <sheet name="NewestWatches" sheetId="9" r:id="rId7"/>
+    <sheet name="CompareHotspots" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>Google</t>
   </si>
@@ -83,6 +85,12 @@
   </si>
   <si>
     <t>Shop Apple tablets</t>
+  </si>
+  <si>
+    <t>Newest</t>
+  </si>
+  <si>
+    <t>Compare Phones &amp; Devices</t>
   </si>
 </sst>
 </file>
@@ -123,10 +131,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,7 +621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7505121-C4A8-6E43-B005-E9FA764849C8}">
   <dimension ref="A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -629,4 +638,69 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988DFD77-1CCF-EE4E-92DB-C30DD4A9A8CD}">
+  <dimension ref="A2:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3320CDE-3A90-1049-BBCA-6D50E0258DA6}">
+  <dimension ref="A2:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="2" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="10.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
two more permutations for adding to cart
</commit_message>
<xml_diff>
--- a/com.verizon/src/test/resources/test_data_verizon.xlsx
+++ b/com.verizon/src/test/resources/test_data_verizon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.verizon/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B5FFB0-665C-8749-9F9F-9947568B58D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3681386-8F54-584E-B184-C3A60484C4E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16060" activeTab="7" xr2:uid="{98B19BF0-E3A6-844B-87BE-D61402A4F806}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16060" activeTab="3" xr2:uid="{98B19BF0-E3A6-844B-87BE-D61402A4F806}"/>
   </bookViews>
   <sheets>
     <sheet name="Google5GPhones" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
   <si>
     <t>Google</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Compare Phones &amp; Devices</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
 </sst>
 </file>
@@ -513,10 +516,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36D147A-E162-B54D-A1C4-FABABDCAA153}">
-  <dimension ref="A2:F3"/>
+  <dimension ref="A2:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -565,6 +568,26 @@
         <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -670,7 +693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3320CDE-3A90-1049-BBCA-6D50E0258DA6}">
   <dimension ref="A2:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
test case write a review passed
</commit_message>
<xml_diff>
--- a/com.verizon/src/test/resources/test_data_verizon.xlsx
+++ b/com.verizon/src/test/resources/test_data_verizon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.verizon/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3681386-8F54-584E-B184-C3A60484C4E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8AACF1-139C-B04F-9A7D-BEFF34D5EA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16060" activeTab="3" xr2:uid="{98B19BF0-E3A6-844B-87BE-D61402A4F806}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16060" firstSheet="1" activeTab="9" xr2:uid="{98B19BF0-E3A6-844B-87BE-D61402A4F806}"/>
   </bookViews>
   <sheets>
     <sheet name="Google5GPhones" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,8 @@
     <sheet name="AppleTablets" sheetId="8" r:id="rId6"/>
     <sheet name="NewestWatches" sheetId="9" r:id="rId7"/>
     <sheet name="CompareHotspots" sheetId="10" r:id="rId8"/>
+    <sheet name="SteelSeriesHeadset" sheetId="11" r:id="rId9"/>
+    <sheet name="WriteAReview" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
   <si>
     <t>Google</t>
   </si>
@@ -94,13 +96,31 @@
   </si>
   <si>
     <t>6</t>
+  </si>
+  <si>
+    <t>SteelSeries</t>
+  </si>
+  <si>
+    <t>Post Review</t>
+  </si>
+  <si>
+    <t>Great Design!</t>
+  </si>
+  <si>
+    <t>The Dynamic Island is very sleek!</t>
+  </si>
+  <si>
+    <t>Adil</t>
+  </si>
+  <si>
+    <t>adilkhaleque429@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -112,6 +132,14 @@
       <sz val="11"/>
       <name val="Menlo"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,16 +159,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -471,6 +502,49 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6195229E-3CFB-2C43-BB76-B2A3D0EF0C72}">
+  <dimension ref="A2:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="25.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{7B8B6B19-D693-9545-BD44-AC39838F2085}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B1DF1D1-FECE-D541-9CCC-DEE78ACD0A7C}">
   <dimension ref="A2"/>
@@ -518,7 +592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36D147A-E162-B54D-A1C4-FABABDCAA153}">
   <dimension ref="A2:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -726,4 +800,24 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33F85A8C-2D51-F04A-9C5C-4497E354C62D}">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test find a store passed
</commit_message>
<xml_diff>
--- a/com.verizon/src/test/resources/test_data_verizon.xlsx
+++ b/com.verizon/src/test/resources/test_data_verizon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.verizon/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDF63B5-6183-084F-8AFB-B1CF3527C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EED8F20-823C-8944-8D39-7E206E7F64EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16060" firstSheet="1" activeTab="10" xr2:uid="{98B19BF0-E3A6-844B-87BE-D61402A4F806}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16060" firstSheet="2" activeTab="11" xr2:uid="{98B19BF0-E3A6-844B-87BE-D61402A4F806}"/>
   </bookViews>
   <sheets>
     <sheet name="Google5GPhones" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="SteelSeriesHeadset" sheetId="11" r:id="rId9"/>
     <sheet name="WriteAReview" sheetId="12" r:id="rId10"/>
     <sheet name="Language" sheetId="13" r:id="rId11"/>
+    <sheet name="StoreLocation" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>Google</t>
   </si>
@@ -118,6 +119,9 @@
   </si>
   <si>
     <t>Business | FRANCE</t>
+  </si>
+  <si>
+    <t>New York, NY</t>
   </si>
 </sst>
 </file>
@@ -553,7 +557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8386FA4A-2740-C14B-9E5A-EB1150A6CBE8}">
   <dimension ref="A2:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -570,6 +574,34 @@
       </c>
       <c r="B2" s="3" t="s">
         <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{016DFC47-46D3-0E4D-B381-EAAA09E7991E}">
+  <dimension ref="A2:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="16.5" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>11102</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test case 15 setup
</commit_message>
<xml_diff>
--- a/com.verizon/src/test/resources/test_data_verizon.xlsx
+++ b/com.verizon/src/test/resources/test_data_verizon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.verizon/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EED8F20-823C-8944-8D39-7E206E7F64EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5760A0C4-B8B5-7D4B-ABBC-5475BC31D337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16060" firstSheet="2" activeTab="11" xr2:uid="{98B19BF0-E3A6-844B-87BE-D61402A4F806}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16060" firstSheet="3" activeTab="12" xr2:uid="{98B19BF0-E3A6-844B-87BE-D61402A4F806}"/>
   </bookViews>
   <sheets>
     <sheet name="Google5GPhones" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="WriteAReview" sheetId="12" r:id="rId10"/>
     <sheet name="Language" sheetId="13" r:id="rId11"/>
     <sheet name="StoreLocation" sheetId="14" r:id="rId12"/>
+    <sheet name="ContactSales" sheetId="15" r:id="rId13"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>Google</t>
   </si>
@@ -122,6 +123,27 @@
   </si>
   <si>
     <t>New York, NY</t>
+  </si>
+  <si>
+    <t>us</t>
+  </si>
+  <si>
+    <t>10-19</t>
+  </si>
+  <si>
+    <t>Advanced_Communications</t>
+  </si>
+  <si>
+    <t>technology</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>Submit</t>
   </si>
 </sst>
 </file>
@@ -585,7 +607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{016DFC47-46D3-0E4D-B381-EAAA09E7991E}">
   <dimension ref="A2:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
@@ -602,6 +624,48 @@
       </c>
       <c r="B2" s="3" t="s">
         <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B45B375-EEC2-2140-A9DD-6323E7C6E071}">
+  <dimension ref="A2:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="A2:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="29.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test case 15 passed
</commit_message>
<xml_diff>
--- a/com.verizon/src/test/resources/test_data_verizon.xlsx
+++ b/com.verizon/src/test/resources/test_data_verizon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.verizon/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5760A0C4-B8B5-7D4B-ABBC-5475BC31D337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53C60D7-74BF-8845-B5DA-DB8E4E9F3FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16060" firstSheet="3" activeTab="12" xr2:uid="{98B19BF0-E3A6-844B-87BE-D61402A4F806}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
   <si>
     <t>Google</t>
   </si>
@@ -144,6 +144,21 @@
   </si>
   <si>
     <t>Submit</t>
+  </si>
+  <si>
+    <t>3825 Corlear Ave Basement 1</t>
+  </si>
+  <si>
+    <t>Khaleque</t>
+  </si>
+  <si>
+    <t>Name of Company</t>
+  </si>
+  <si>
+    <t>Bronx</t>
+  </si>
+  <si>
+    <t>You can provide some good internet.</t>
   </si>
 </sst>
 </file>
@@ -633,19 +648,30 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B45B375-EEC2-2140-A9DD-6323E7C6E071}">
-  <dimension ref="A2:G2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="A2:G2"/>
+  <dimension ref="A2:P2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="29.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="1" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="29.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="2"/>
+    <col min="6" max="6" width="26.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="28" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="2"/>
+    <col min="11" max="11" width="28.1640625" style="2" customWidth="1"/>
+    <col min="12" max="14" width="10.83203125" style="2"/>
+    <col min="15" max="15" width="31.6640625" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
@@ -659,16 +685,46 @@
         <v>28</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="2">
+        <v>2111111111</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="K2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="N2" s="2">
+        <v>10463</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{A8BC0A95-A4F8-A943-A0DD-09E9297D91C6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>